<commit_message>
Energy Balance Test Update
</commit_message>
<xml_diff>
--- a/Structure/1 - Whole System/EnBalanceData.xlsx
+++ b/Structure/1 - Whole System/EnBalanceData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\ENERGY BRANCH\Statistics\R Shiny\Reorganised\Structure\1 - Whole System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ische\Documents\Github\SESH\Structure\1 - Whole System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1382EF6-C227-4244-B115-E796F8475F13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8D4337-32E8-4162-B0C8-E1B4AB140BAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{77BAC818-DF8C-46E9-B076-3CA836B62C5B}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -607,7 +608,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J28"/>
+      <selection activeCell="B5" sqref="B5:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,22 +704,22 @@
         <v>13</v>
       </c>
       <c r="B5" s="15">
-        <v>507.44028852584307</v>
+        <v>401.93995414158786</v>
       </c>
       <c r="C5" s="15">
-        <v>48589.840699024528</v>
+        <v>52926.146686182503</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="16">
-        <v>24954.6563307059</v>
+        <v>24122.958278160062</v>
       </c>
       <c r="F5" s="16">
-        <v>845.39852171455186</v>
+        <v>757.20375649635287</v>
       </c>
       <c r="G5" s="15">
-        <v>5786.0209006781306</v>
+        <v>5034.0136633455586</v>
       </c>
       <c r="H5" s="15" t="s">
         <v>14</v>
@@ -727,7 +728,7 @@
         <v>14</v>
       </c>
       <c r="J5" s="15">
-        <v>80683.35674064896</v>
+        <v>83242.262338326065</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -735,31 +736,31 @@
         <v>15</v>
       </c>
       <c r="B6" s="15">
-        <v>8.7004155918601298E-6</v>
+        <v>3.3916809974204643E-5</v>
       </c>
       <c r="C6" s="15">
-        <v>5377.4142107157004</v>
+        <v>6090.2525177746411</v>
       </c>
       <c r="D6" s="15">
-        <v>2967.9976667947853</v>
+        <v>3176.6055366253076</v>
       </c>
       <c r="E6" s="16">
-        <v>14091.653365434298</v>
+        <v>14063.185452902055</v>
       </c>
       <c r="F6" s="16">
-        <v>227.33523256795777</v>
+        <v>241.11632141442743</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="15">
-        <v>119.63693035253721</v>
+        <v>99.635167669819978</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="15">
-        <v>22784.037414565697</v>
+        <v>23670.795030303067</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -770,13 +771,13 @@
         <v>14</v>
       </c>
       <c r="C7" s="13">
-        <v>5377.4142107157004</v>
+        <v>6090.2525177746411</v>
       </c>
       <c r="D7" s="13">
-        <v>2249.3242418032173</v>
+        <v>2446.5685462545644</v>
       </c>
       <c r="E7" s="13">
-        <v>14051.676698194402</v>
+        <v>14051.762682717188</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>14</v>
@@ -805,10 +806,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="13">
-        <v>718.67342499156814</v>
+        <v>730.03699037074352</v>
       </c>
       <c r="E8" s="17">
-        <v>39.97666723989704</v>
+        <v>11.422770184866787</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>14</v>
@@ -817,7 +818,7 @@
         <v>14</v>
       </c>
       <c r="H8" s="13">
-        <v>119.63693035253721</v>
+        <v>99.635167669819978</v>
       </c>
       <c r="I8" s="13" t="s">
         <v>14</v>
@@ -831,31 +832,31 @@
         <v>18</v>
       </c>
       <c r="B9" s="15">
-        <v>-365.33074165217158</v>
+        <v>-275.65451944274798</v>
       </c>
       <c r="C9" s="15">
-        <v>-42065.105302522512</v>
+        <v>-47955.704136857777</v>
       </c>
       <c r="D9" s="15">
-        <v>-6710.5260209438939</v>
+        <v>-5979.4983924660055</v>
       </c>
       <c r="E9" s="16">
-        <v>-30219.38193800786</v>
+        <v>-28722.282377307893</v>
       </c>
       <c r="F9" s="16">
-        <v>-28.201536535983525</v>
+        <v>-16.021582286988252</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="15">
-        <v>-1226.1036973344865</v>
+        <v>-1261.8843508168598</v>
       </c>
       <c r="I9" s="15" t="s">
         <v>14</v>
       </c>
       <c r="J9" s="15">
-        <v>-80614.649236996906</v>
+        <v>-84211.045359178286</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -866,13 +867,13 @@
         <v>14</v>
       </c>
       <c r="C10" s="13">
-        <v>-22245.008546123943</v>
+        <v>-22787.404014714884</v>
       </c>
       <c r="D10" s="13">
-        <v>-5607.2990068710478</v>
+        <v>-5596.7122406302451</v>
       </c>
       <c r="E10" s="17">
-        <v>-1679.111265264949</v>
+        <v>-1679.1112652649533</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>14</v>
@@ -898,13 +899,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="13">
-        <v>-19820.096756398569</v>
+        <v>-25168.300122142897</v>
       </c>
       <c r="D11" s="13">
-        <v>-1103.2270140728463</v>
+        <v>-382.78615183576028</v>
       </c>
       <c r="E11" s="17">
-        <v>-28540.27067274291</v>
+        <v>-27043.171112042939</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>14</v>
@@ -913,7 +914,7 @@
         <v>14</v>
       </c>
       <c r="H11" s="13">
-        <v>-1226.1036973344865</v>
+        <v>-1261.8843508168598</v>
       </c>
       <c r="I11" s="13" t="s">
         <v>14</v>
@@ -933,7 +934,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="15">
-        <v>-972.4461777555448</v>
+        <v>-1002.590149267652</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>14</v>
@@ -951,7 +952,7 @@
         <v>14</v>
       </c>
       <c r="J12" s="15">
-        <v>-972.4461777555448</v>
+        <v>-1002.590149267652</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -962,10 +963,10 @@
         <v>0</v>
       </c>
       <c r="C13" s="15">
-        <v>51.437059283466994</v>
+        <v>44.849882055171939</v>
       </c>
       <c r="D13" s="15">
-        <v>-19.073019937128301</v>
+        <v>44.719879280166758</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>14</v>
@@ -983,7 +984,7 @@
         <v>14</v>
       </c>
       <c r="J13" s="15">
-        <v>32.364039346338693</v>
+        <v>89.569761335338697</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -991,31 +992,31 @@
         <v>21</v>
       </c>
       <c r="B14" s="19">
-        <v>142.1095555740871</v>
+        <v>126.28546861564988</v>
       </c>
       <c r="C14" s="19">
-        <v>11953.586666501185</v>
+        <v>11105.544949154541</v>
       </c>
       <c r="D14" s="19">
-        <v>-4734.0475518417816</v>
+        <v>-3760.7631258281831</v>
       </c>
       <c r="E14" s="20">
-        <v>8826.9277581323367</v>
+        <v>9463.861353754226</v>
       </c>
       <c r="F14" s="20">
-        <v>1044.5328718620462</v>
+        <v>981.73236197407516</v>
       </c>
       <c r="G14" s="19">
-        <v>5786.0209006781306</v>
+        <v>5034.0136633455586</v>
       </c>
       <c r="H14" s="19">
-        <v>-1106.4667669819491</v>
+        <v>-1162.2491831470397</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>14</v>
       </c>
       <c r="J14" s="19">
-        <v>21912.663433924055</v>
+        <v>21788.425487868826</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1026,13 +1027,13 @@
         <v>0</v>
       </c>
       <c r="C15" s="19">
-        <v>1.4033817365998402E-2</v>
+        <v>0</v>
       </c>
       <c r="D15" s="19">
-        <v>-0.69716244745268341</v>
+        <v>-1.1240450149512071</v>
       </c>
       <c r="E15" s="16">
-        <v>8.5984522786020534E-2</v>
+        <v>0</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>14</v>
@@ -1041,13 +1042,13 @@
         <v>14</v>
       </c>
       <c r="H15" s="15">
-        <v>7.0768701633717228</v>
+        <v>0</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>14</v>
       </c>
       <c r="J15" s="15">
-        <v>6.4797260560710583</v>
+        <v>-1.1240450149512071</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1055,31 +1056,31 @@
         <v>23</v>
       </c>
       <c r="B16" s="19">
-        <v>142.1095555740871</v>
+        <v>126.28546861564988</v>
       </c>
       <c r="C16" s="19">
-        <v>11953.572632683819</v>
+        <v>11105.544949154537</v>
       </c>
       <c r="D16" s="19">
-        <v>-4734.7447142892343</v>
+        <v>-3761.8871708431343</v>
       </c>
       <c r="E16" s="20">
-        <v>8827.0137426551228</v>
+        <v>9463.8613537542296</v>
       </c>
       <c r="F16" s="20">
-        <v>1044.5328718620462</v>
+        <v>981.73236197407516</v>
       </c>
       <c r="G16" s="19">
-        <v>5786.0209006781306</v>
+        <v>5034.0136633455586</v>
       </c>
       <c r="H16" s="19">
-        <v>-1099.3898968185774</v>
+        <v>-1162.2491831470397</v>
       </c>
       <c r="I16" s="19" t="s">
         <v>14</v>
       </c>
       <c r="J16" s="19">
-        <v>21919.115092345393</v>
+        <v>21787.301442853874</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1090,10 +1091,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="15">
-        <v>-2559.5052509966904</v>
+        <v>-1930.4810265331166</v>
       </c>
       <c r="D17" s="15">
-        <v>2559.5052509966904</v>
+        <v>1930.4810265331166</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>14</v>
@@ -1102,10 +1103,10 @@
         <v>14</v>
       </c>
       <c r="G17" s="15">
-        <v>-1952.9624355017334</v>
+        <v>-2092.7724080189364</v>
       </c>
       <c r="H17" s="15">
-        <v>1952.9624355017334</v>
+        <v>2092.7724080189364</v>
       </c>
       <c r="I17" s="15" t="s">
         <v>14</v>
@@ -1122,28 +1123,28 @@
         <v>0</v>
       </c>
       <c r="C18" s="15">
-        <v>-9394.0673816871295</v>
+        <v>-9175.0639226214207</v>
       </c>
       <c r="D18" s="15">
-        <v>9071.6297832178334</v>
+        <v>8940.7948701448513</v>
       </c>
       <c r="E18" s="15">
-        <v>-962.87537035222795</v>
+        <v>-1478.3858772496594</v>
       </c>
       <c r="F18" s="15">
-        <v>-624.70011117190791</v>
+        <v>-544.66443420107191</v>
       </c>
       <c r="G18" s="15">
-        <v>-3833.0584651763975</v>
+        <v>-2941.2412553266217</v>
       </c>
       <c r="H18" s="15">
-        <v>2232.5687644510422</v>
+        <v>2054.8110221894326</v>
       </c>
       <c r="I18" s="15">
-        <v>121.41584435849438</v>
+        <v>118.85195238779175</v>
       </c>
       <c r="J18" s="15">
-        <v>-3389.0869363602924</v>
+        <v>-3024.8976446766983</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1157,25 +1158,25 @@
         <v>14</v>
       </c>
       <c r="D19" s="13">
-        <v>-213.22914566160273</v>
+        <v>-122.20203054151465</v>
       </c>
       <c r="E19" s="13">
-        <v>-778.00251947731238</v>
+        <v>-1296.428062330529</v>
       </c>
       <c r="F19" s="13">
-        <v>-611.64823405715549</v>
+        <v>-533.195107588528</v>
       </c>
       <c r="G19" s="13">
-        <v>-3833.0584651763975</v>
+        <v>-2941.2412553266217</v>
       </c>
       <c r="H19" s="13">
-        <v>2232.5687644510422</v>
+        <v>2054.8110221894326</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>14</v>
       </c>
       <c r="J19" s="13">
-        <v>-3203.3695999214265</v>
+        <v>-2838.2554335977607</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1186,10 +1187,10 @@
         <v>14</v>
       </c>
       <c r="C20" s="13">
-        <v>-9394.0673816871295</v>
+        <v>-9175.0639226214207</v>
       </c>
       <c r="D20" s="13">
-        <v>9354.209237177869</v>
+        <v>9125.3215529965692</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>14</v>
@@ -1207,7 +1208,7 @@
         <v>14</v>
       </c>
       <c r="J20" s="13">
-        <v>-39.858144509260455</v>
+        <v>-49.742369624851563</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1221,13 +1222,13 @@
         <v>14</v>
       </c>
       <c r="D21" s="13">
-        <v>-69.350308298432026</v>
+        <v>-62.324652310203362</v>
       </c>
       <c r="E21" s="13">
-        <v>-184.87285087491563</v>
+        <v>-181.95781491913053</v>
       </c>
       <c r="F21" s="13">
-        <v>-13.051877114752415</v>
+        <v>-11.46932661254391</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>14</v>
@@ -1236,10 +1237,10 @@
         <v>14</v>
       </c>
       <c r="I21" s="13">
-        <v>121.41584435849438</v>
+        <v>118.85195238779175</v>
       </c>
       <c r="J21" s="13">
-        <v>-145.85919192960569</v>
+        <v>-136.89984145408604</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1253,10 +1254,10 @@
         <v>14</v>
       </c>
       <c r="D22" s="15">
-        <v>592.27299800725962</v>
+        <v>581.86315444322327</v>
       </c>
       <c r="E22" s="15">
-        <v>3615.8056201903792</v>
+        <v>3761.5887271162856</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>14</v>
@@ -1265,13 +1266,13 @@
         <v>14</v>
       </c>
       <c r="H22" s="15">
-        <v>455.85862543396365</v>
+        <v>430.6151697031857</v>
       </c>
       <c r="I22" s="15">
-        <v>25.751311415458161</v>
+        <v>30.554445938952057</v>
       </c>
       <c r="J22" s="15">
-        <v>4689.6885550470606</v>
+        <v>4804.6214972016469</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1279,31 +1280,31 @@
         <v>30</v>
       </c>
       <c r="B23" s="19">
-        <v>142.1095555740871</v>
+        <v>126.28546861564988</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="19">
-        <v>6304.1173219180291</v>
+        <v>6527.5255713916094</v>
       </c>
       <c r="E23" s="19">
-        <v>4248.3327521125166</v>
+        <v>4223.8867493882835</v>
       </c>
       <c r="F23" s="19">
-        <v>419.83276069013823</v>
+        <v>437.06792777300325</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>14</v>
       </c>
       <c r="H23" s="19">
-        <v>2630.2826777002342</v>
+        <v>2554.7190773581437</v>
       </c>
       <c r="I23" s="19">
-        <v>95.664532943036221</v>
+        <v>88.297506448839698</v>
       </c>
       <c r="J23" s="19">
-        <v>13840.339600938039</v>
+        <v>13957.78230097553</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1317,10 +1318,10 @@
         <v>14</v>
       </c>
       <c r="D24" s="13">
-        <v>1038.9119930141237</v>
+        <v>1125.2647513822537</v>
       </c>
       <c r="E24" s="13">
-        <v>60.93324677558072</v>
+        <v>59.263883971473689</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>14</v>
@@ -1332,10 +1333,10 @@
         <v>14</v>
       </c>
       <c r="I24" s="13">
-        <v>61.272933863648511</v>
+        <v>52.619899118795843</v>
       </c>
       <c r="J24" s="13">
-        <v>1161.1181736533529</v>
+        <v>1237.1485344725234</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1343,31 +1344,31 @@
         <v>32</v>
       </c>
       <c r="B25" s="13">
-        <v>93.280083568398254</v>
+        <v>80.37196056133088</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="13">
-        <v>357.81481657388258</v>
+        <v>177.56837512603184</v>
       </c>
       <c r="E25" s="13">
-        <v>895.70385173293903</v>
+        <v>935.55392882101103</v>
       </c>
       <c r="F25" s="13">
-        <v>79.380273003241854</v>
+        <v>98.132461902953565</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H25" s="13">
-        <v>730.47154133671813</v>
+        <v>714.94006808840356</v>
       </c>
       <c r="I25" s="13">
-        <v>9.8974895872053352</v>
+        <v>9.4953201417375954</v>
       </c>
       <c r="J25" s="13">
-        <v>2166.5480558023851</v>
+        <v>2016.0621146414685</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1375,31 +1376,31 @@
         <v>33</v>
       </c>
       <c r="B26" s="13">
-        <v>45.931319073176653</v>
+        <v>43.430782459157591</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="13">
-        <v>263.24567172082999</v>
+        <v>263.14447083901541</v>
       </c>
       <c r="E26" s="13">
-        <v>2437.826076868796</v>
+        <v>2355.44966903881</v>
       </c>
       <c r="F26" s="13">
-        <v>151.39981736084357</v>
+        <v>160.10730182375826</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H26" s="13">
-        <v>1090.4646125001088</v>
+        <v>1059.1373970396792</v>
       </c>
       <c r="I26" s="13">
-        <v>24.494109492182364</v>
+        <v>26.182287188306248</v>
       </c>
       <c r="J26" s="13">
-        <v>4013.3616070159369</v>
+        <v>3907.4519083887267</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1407,31 +1408,31 @@
         <v>34</v>
       </c>
       <c r="B27" s="13">
-        <v>0.32053293805785971</v>
+        <v>0.36113499570077584</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="13">
-        <v>4376.0488430404521</v>
+        <v>4449.0157472838027</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="13">
-        <v>68.122607640065851</v>
+        <v>92.185039969441235</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="13">
-        <v>37.716437475378008</v>
+        <v>38.348248213293964</v>
       </c>
       <c r="I27" s="13" t="s">
         <v>14</v>
       </c>
       <c r="J27" s="13">
-        <v>4482.2084210939547</v>
+        <v>4579.910170462239</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1439,31 +1440,31 @@
         <v>35</v>
       </c>
       <c r="B28" s="13">
-        <v>2.5776199944543379</v>
+        <v>2.1129921471820268</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="13">
-        <v>268.09599756874275</v>
+        <v>512.53222676050734</v>
       </c>
       <c r="E28" s="13">
-        <v>853.86957673520146</v>
+        <v>873.61926755698801</v>
       </c>
       <c r="F28" s="13">
-        <v>120.93006268598701</v>
+        <v>86.643124076850185</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="13">
-        <v>771.63008638802933</v>
+        <v>742.29336401676699</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>14</v>
       </c>
       <c r="J28" s="13">
-        <v>2017.1033433724147</v>
+        <v>2217.2009745582945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>